<commit_message>
changed name of variables in MergeSort Algorithm for better understanding
</commit_message>
<xml_diff>
--- a/Google/GoogleInterview.xlsx
+++ b/Google/GoogleInterview.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luis/MyDocuments/Google/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SourceCode\Git-P\Practice\Practice\Google\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A9484E-45B6-834E-88A6-69E46BE8A773}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10240" windowHeight="18000" xr2:uid="{1604A2A1-32AD-A043-9628-9506C1A73692}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10236" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,7 +106,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -133,12 +132,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -153,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -161,14 +166,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -483,117 +491,117 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD1E0825-899A-BE47-9721-7BFAB078F06B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" customWidth="1"/>
-    <col min="2" max="2" width="53.83203125" customWidth="1"/>
+    <col min="1" max="1" width="27.796875" customWidth="1"/>
+    <col min="2" max="2" width="53.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-    </row>
-    <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="B1" s="5"/>
+    </row>
+    <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
       <c r="B11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
       <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
       <c r="B13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
       <c r="B14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
+    <row r="15" spans="1:2" ht="78" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
+    <row r="16" spans="1:2" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:2" ht="78" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
+    <row r="18" spans="1:2" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Completed Walking on Clouds HackerRank Warm-Up Exercise
</commit_message>
<xml_diff>
--- a/Google/GoogleInterview.xlsx
+++ b/Google/GoogleInterview.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SourceCode\Git-P\Practice\Practice\Google\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SourceCode\Git-P\Practice\Google\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -169,13 +169,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -494,7 +494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -505,10 +505,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -519,12 +519,12 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
@@ -557,43 +557,43 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="B11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
+      <c r="A12" s="5"/>
       <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
+      <c r="A13" s="5"/>
       <c r="B13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
+      <c r="A14" s="5"/>
       <c r="B14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="78" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="78" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -601,7 +601,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
+      <c r="A18" s="5"/>
       <c r="B18" s="1" t="s">
         <v>18</v>
       </c>

</xml_diff>